<commit_message>
Add fruit sales Excel file
</commit_message>
<xml_diff>
--- a/fruit_sales_20250808.xlsx
+++ b/fruit_sales_20250808.xlsx
@@ -448,51 +448,47 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mangos</t>
+          <t>manos</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Bananas</t>
-        </is>
-      </c>
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Pineapples</t>
+          <t>fjef</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Apples</t>
+          <t>fefes</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Grapes</t>
+          <t>ffsfsd</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>